<commit_message>
:beetle: previous set had an error due to Excel dragging
</commit_message>
<xml_diff>
--- a/smallworld/mergers.xlsx
+++ b/smallworld/mergers.xlsx
@@ -14,7 +14,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="149">
+  <si>
+    <t>comRMSD</t>
+  </si>
+  <si>
+    <t>N_hits</t>
+  </si>
+  <si>
+    <t>∆∆G</t>
+  </si>
+  <si>
+    <t>N_diff_atoms</t>
+  </si>
+  <si>
+    <t>LE</t>
+  </si>
+  <si>
+    <t>N_constrained_atoms</t>
+  </si>
+  <si>
+    <t>%Rank</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
   <si>
     <t>original SMILES</t>
   </si>
@@ -22,34 +46,88 @@
     <t>regarded</t>
   </si>
   <si>
-    <t>N_diff_atoms</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>N_hits</t>
-  </si>
-  <si>
-    <t>LE</t>
-  </si>
-  <si>
-    <t>comRMSD</t>
+    <t>disregarded</t>
   </si>
   <si>
     <t>method</t>
   </si>
   <si>
-    <t>N_constrained_atoms</t>
-  </si>
-  <si>
-    <t>%Rank</t>
-  </si>
-  <si>
-    <t>disregarded</t>
-  </si>
-  <si>
-    <t>∆∆G</t>
+    <t>0.2567963687437966</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>-9.023928517525322</t>
+  </si>
+  <si>
+    <t>-0.3759970215635551</t>
+  </si>
+  <si>
+    <t>24.0</t>
+  </si>
+  <si>
+    <t>5.555555555555555</t>
+  </si>
+  <si>
+    <t>s-11-11560436-10336618</t>
+  </si>
+  <si>
+    <t>O=C1CSC2=CC(C(=O)OC3C4=CC=CC=C4CC3F)=CC=C2N1</t>
+  </si>
+  <si>
+    <t>mac-x0213,mac-x0380</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>nan</t>
+  </si>
+  <si>
+    <t>0.23898978092089074</t>
+  </si>
+  <si>
+    <t>-8.280124917397782</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>-0.31846634297683774</t>
+  </si>
+  <si>
+    <t>26.0</t>
+  </si>
+  <si>
+    <t>11.11111111111111</t>
+  </si>
+  <si>
+    <t>m-272610-18205366-17773864</t>
+  </si>
+  <si>
+    <t>O=C1CSC2=CC(C(=O)NC3C4=CC=CC=C4CC3C(=O)O)=CC=C2N1</t>
+  </si>
+  <si>
+    <t>0.35276879316142956</t>
+  </si>
+  <si>
+    <t>-6.805870090606924</t>
+  </si>
+  <si>
+    <t>7.0</t>
+  </si>
+  <si>
+    <t>-0.32408905193366305</t>
+  </si>
+  <si>
+    <t>21.0</t>
+  </si>
+  <si>
+    <t>16.666666666666664</t>
+  </si>
+  <si>
+    <t>s-487-210243-12883856</t>
   </si>
   <si>
     <t>O=C(NC1=CC=CN=C1)NC2=CC=C3C=CC=CC3=N2</t>
@@ -58,361 +136,331 @@
     <t>mac-x0341,diamond-x0128_0_A</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>s-487-210243-12883856</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>-0.35231190473093843</t>
-  </si>
-  <si>
-    <t>0.3507061753499238</t>
-  </si>
-  <si>
-    <t>nan</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>6.666666666666667</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>-7.398549999349707</t>
-  </si>
-  <si>
-    <t>O=C1CSC2=CC(C(=O)NC3C4=CC=CC=C4CC3C(=O)O)=CC=C2N1</t>
-  </si>
-  <si>
-    <t>mac-x0213,mac-x0380</t>
-  </si>
-  <si>
-    <t>-1</t>
-  </si>
-  <si>
-    <t>m-272610-18205366-17773864</t>
-  </si>
-  <si>
-    <t>-0.2995769867850402</t>
-  </si>
-  <si>
-    <t>0.5521480431355901</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>13.333333333333334</t>
-  </si>
-  <si>
-    <t>-8.088578643196085</t>
+    <t>0.5267832717395411</t>
+  </si>
+  <si>
+    <t>-7.6858563378019</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>-0.307434253512076</t>
+  </si>
+  <si>
+    <t>25.0</t>
+  </si>
+  <si>
+    <t>22.22222222222222</t>
+  </si>
+  <si>
+    <t>m-272610-18205442-17773864</t>
+  </si>
+  <si>
+    <t>O=C1CSC2=CC(C(=O)N3C4=CC=CC=C4C[C@@H]3C(=O)O)=CC=C2N1</t>
+  </si>
+  <si>
+    <t>0.218117838115886</t>
+  </si>
+  <si>
+    <t>-10.862739604544958</t>
+  </si>
+  <si>
+    <t>-5.0</t>
+  </si>
+  <si>
+    <t>-0.38795498587660565</t>
+  </si>
+  <si>
+    <t>23.0</t>
+  </si>
+  <si>
+    <t>27.77777777777778</t>
+  </si>
+  <si>
+    <t>m-272610-18205366-17768894</t>
+  </si>
+  <si>
+    <t>O=C(NC1C2=CC=CC=C2CC1C(=O)O)C1=CC=C(NC(=O)C2CC2)C=C1</t>
+  </si>
+  <si>
+    <t>mac-x0213,mac-x0398</t>
+  </si>
+  <si>
+    <t>0.5416381567588668</t>
+  </si>
+  <si>
+    <t>-8.923281899936448</t>
+  </si>
+  <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>-0.38796877825810644</t>
+  </si>
+  <si>
+    <t>33.33333333333333</t>
+  </si>
+  <si>
+    <t>m-2430-8961378-14047914</t>
+  </si>
+  <si>
+    <t>CC1=CN=NC=C1NC(=O)NCC2=NC3=CC=CC=C3C(=O)[NH]2</t>
+  </si>
+  <si>
+    <t>0.6017645481652864</t>
+  </si>
+  <si>
+    <t>-5.206435311891445</t>
+  </si>
+  <si>
+    <t>6.0</t>
+  </si>
+  <si>
+    <t>-0.23665615054052022</t>
+  </si>
+  <si>
+    <t>38.88888888888889</t>
+  </si>
+  <si>
+    <t>s-487-14047900-150243</t>
   </si>
   <si>
     <t>O=C(NCC1=NC2=CC=CC=C2C(=O)[NH]1)NC3=CC=CN=C3</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>s-487-14047900-150243</t>
-  </si>
-  <si>
-    <t>-0.2793339075508257</t>
-  </si>
-  <si>
-    <t>0.5547163689670606</t>
-  </si>
-  <si>
-    <t>20.0</t>
-  </si>
-  <si>
-    <t>-6.145345966118166</t>
-  </si>
-  <si>
-    <t>CC1=CN=NC=C1NC(=O)NCC2=NC3=CC=CC=C3C(=O)[NH]2</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>m-2430-8961378-14047914</t>
-  </si>
-  <si>
-    <t>-0.4001048834872237</t>
-  </si>
-  <si>
-    <t>0.533089479221962</t>
-  </si>
-  <si>
-    <t>26.666666666666668</t>
-  </si>
-  <si>
-    <t>-9.202412320206145</t>
+    <t>0.48469744036424633</t>
+  </si>
+  <si>
+    <t>-7.678302020392907</t>
+  </si>
+  <si>
+    <t>-4.0</t>
+  </si>
+  <si>
+    <t>-0.28438155631084844</t>
+  </si>
+  <si>
+    <t>44.44444444444444</t>
+  </si>
+  <si>
+    <t>m-272610-18205366-17770920</t>
   </si>
   <si>
     <t>COC(=O)NC1=CC=C(C(=O)NC2C3=CC=CC=C3CC2C(=O)O)C=C1</t>
   </si>
   <si>
-    <t>mac-x0213,mac-x0398</t>
-  </si>
-  <si>
-    <t>-4</t>
-  </si>
-  <si>
-    <t>m-272610-18205366-17770920</t>
-  </si>
-  <si>
-    <t>-0.404731910961565</t>
-  </si>
-  <si>
-    <t>0.4921695536755777</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>33.33333333333333</t>
-  </si>
-  <si>
-    <t>-10.927761595962256</t>
+    <t>0.5134190592827487</t>
+  </si>
+  <si>
+    <t>-9.906482592195</t>
+  </si>
+  <si>
+    <t>-0.35380294972125</t>
+  </si>
+  <si>
+    <t>50.0</t>
+  </si>
+  <si>
+    <t>m-272610-18205366-18219660</t>
   </si>
   <si>
     <t>CNC(=O)NC1=CC=C(C(=O)NC2C3=CC=CC=C3CC2C(=O)O)C=C1</t>
   </si>
   <si>
-    <t>-5</t>
-  </si>
-  <si>
-    <t>m-272610-18205366-18219660</t>
-  </si>
-  <si>
-    <t>-0.3242844187817063</t>
-  </si>
-  <si>
-    <t>0.42956752771777945</t>
-  </si>
-  <si>
-    <t>40.0</t>
-  </si>
-  <si>
-    <t>-9.079963725887776</t>
+    <t>0.504558739632097</t>
+  </si>
+  <si>
+    <t>-8.254410048311911</t>
+  </si>
+  <si>
+    <t>-6.0</t>
+  </si>
+  <si>
+    <t>-0.28463482925213485</t>
+  </si>
+  <si>
+    <t>55.55555555555556</t>
+  </si>
+  <si>
+    <t>m-272610-18205366-18208686</t>
   </si>
   <si>
     <t>O=C(NC1=CC=C(C(=O)NC2C3=CC=CC=C3CC2C(=O)O)C=C1)NC1CC1</t>
   </si>
   <si>
-    <t>-6</t>
-  </si>
-  <si>
-    <t>m-272610-18205366-18208686</t>
-  </si>
-  <si>
-    <t>-0.36383250599541067</t>
-  </si>
-  <si>
-    <t>0.48293770414718734</t>
-  </si>
-  <si>
-    <t>46.666666666666664</t>
-  </si>
-  <si>
-    <t>-10.55114267386691</t>
-  </si>
-  <si>
-    <t>O=C(NC1C2=CC=CC=C2CC1C(=O)O)C1=CC=C(NC(=O)C2CC2)C=C1</t>
-  </si>
-  <si>
-    <t>m-272610-18205366-17768894</t>
-  </si>
-  <si>
-    <t>-0.2905800384533589</t>
-  </si>
-  <si>
-    <t>0.489135039591851</t>
-  </si>
-  <si>
-    <t>53.333333333333336</t>
-  </si>
-  <si>
-    <t>-8.426821115147408</t>
+    <t>0.5046091470676565</t>
+  </si>
+  <si>
+    <t>-8.149351266258046</t>
+  </si>
+  <si>
+    <t>-8.0</t>
+  </si>
+  <si>
+    <t>-0.26288229891154985</t>
+  </si>
+  <si>
+    <t>61.111111111111114</t>
+  </si>
+  <si>
+    <t>s-188690-16712282-7316554</t>
   </si>
   <si>
     <t>O=C(NC1=CC=C(C(=O)NC2C3=C(CC2C(=O)O)C(O)=CC=C3)C=C1)NC1CC1</t>
   </si>
   <si>
-    <t>-8</t>
-  </si>
-  <si>
-    <t>s-188690-16712282-7316554</t>
-  </si>
-  <si>
-    <t>-0.3018969134286844</t>
-  </si>
-  <si>
-    <t>0.452079927523403</t>
-  </si>
-  <si>
-    <t>60.0</t>
-  </si>
-  <si>
-    <t>-9.358804316289216</t>
+    <t>1.0621444313761892</t>
+  </si>
+  <si>
+    <t>-4.585113076127867</t>
+  </si>
+  <si>
+    <t>-0.1834045230451147</t>
+  </si>
+  <si>
+    <t>19.0</t>
+  </si>
+  <si>
+    <t>66.66666666666666</t>
+  </si>
+  <si>
+    <t>s-34-13231222-1282712-</t>
+  </si>
+  <si>
+    <t>CC1=CC=C(C2=NC(CN3C=NC4=C(N)N=C(N)N=C43)=CS2)O1</t>
+  </si>
+  <si>
+    <t>mac-x0138,mac-x0161</t>
+  </si>
+  <si>
+    <t>1.3412346780256101</t>
+  </si>
+  <si>
+    <t>-1.5026306963677205</t>
+  </si>
+  <si>
+    <t>4.0</t>
+  </si>
+  <si>
+    <t>-0.06260961234865502</t>
+  </si>
+  <si>
+    <t>72.22222222222221</t>
+  </si>
+  <si>
+    <t>s-11-2990918-53482</t>
+  </si>
+  <si>
+    <t>O=C(NC1=NC2=CC=CC=C2C(=O)[NH]1)C3=CC=CN=C3</t>
+  </si>
+  <si>
+    <t>diamond-x0128_0_A,mac-x0341</t>
+  </si>
+  <si>
+    <t>1.7796259906695753</t>
+  </si>
+  <si>
+    <t>-4.370858239090608</t>
+  </si>
+  <si>
+    <t>-0.19867537450411854</t>
+  </si>
+  <si>
+    <t>18.0</t>
+  </si>
+  <si>
+    <t>77.77777777777779</t>
+  </si>
+  <si>
+    <t>s-34-13231222-10902660</t>
+  </si>
+  <si>
+    <t>NC1=NC(N)=C2N=CN(CC3=CSC(Cl)=N3)C2=N1</t>
+  </si>
+  <si>
+    <t>1.6426282124828018</t>
+  </si>
+  <si>
+    <t>-5.612434660174012</t>
+  </si>
+  <si>
+    <t>-0.255110666371546</t>
+  </si>
+  <si>
+    <t>17.0</t>
+  </si>
+  <si>
+    <t>83.33333333333334</t>
+  </si>
+  <si>
+    <t>s-34-13231222-7874778</t>
+  </si>
+  <si>
+    <t>NC1=NC(N)=C2N=CN(CC3=CSC(C4CC4)=N3)C2=N1</t>
+  </si>
+  <si>
+    <t>2.0860609877097183</t>
+  </si>
+  <si>
+    <t>-5.738431669608091</t>
+  </si>
+  <si>
+    <t>-0.2732586509337186</t>
+  </si>
+  <si>
+    <t>88.88888888888889</t>
+  </si>
+  <si>
+    <t>s-34-13231222-13910464</t>
   </si>
   <si>
     <t>CC1=NC(CN2C=NC3=C(N)N=C(N)N=C32)=CS1</t>
   </si>
   <si>
-    <t>mac-x0138</t>
-  </si>
-  <si>
-    <t>s-34-13231222-13910464</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>-0.5484581487386703</t>
-  </si>
-  <si>
-    <t>0.29013789824840186</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>66.66666666666666</t>
-  </si>
-  <si>
-    <t>mac-x0159</t>
-  </si>
-  <si>
-    <t>-9.872246677296065</t>
-  </si>
-  <si>
-    <t>O=C(NC1=NC2=CC=CC=C2C(=O)[NH]1)C3=CC=CN=C3</t>
-  </si>
-  <si>
-    <t>diamond-x0128_0_A</t>
-  </si>
-  <si>
-    <t>s-11-2990918-53482</t>
-  </si>
-  <si>
-    <t>-0.08031607805625891</t>
-  </si>
-  <si>
-    <t>1.1970490800297204</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>73.33333333333333</t>
-  </si>
-  <si>
-    <t>mac-x0341</t>
-  </si>
-  <si>
-    <t>-1.7669537172376961</t>
+    <t>2.735909451976027</t>
+  </si>
+  <si>
+    <t>-1.954573078152455</t>
+  </si>
+  <si>
+    <t>-3.0</t>
+  </si>
+  <si>
+    <t>-0.07517588762124827</t>
+  </si>
+  <si>
+    <t>16.0</t>
+  </si>
+  <si>
+    <t>94.44444444444444</t>
+  </si>
+  <si>
+    <t>m-272610-18205366-9959790</t>
+  </si>
+  <si>
+    <t>O=C(NC1C2=CC=CC=C2CC1C(=O)O)C3=CC=CC=C3</t>
+  </si>
+  <si>
+    <t>2.065304552538642</t>
+  </si>
+  <si>
+    <t>-4.326511482482654</t>
+  </si>
+  <si>
+    <t>-0.18027131177011058</t>
+  </si>
+  <si>
+    <t>12.0</t>
+  </si>
+  <si>
+    <t>100.0</t>
+  </si>
+  <si>
+    <t>s-22-17541880-294410</t>
   </si>
   <si>
     <t>O=C(CC1=CC=NC=C1)NC2=NC3=CC=CC=C3C(=O)[NH]2</t>
-  </si>
-  <si>
-    <t>-9</t>
-  </si>
-  <si>
-    <t>s-22-17541880-294410</t>
-  </si>
-  <si>
-    <t>-0.23498488953626503</t>
-  </si>
-  <si>
-    <t>0.25798643375185454</t>
-  </si>
-  <si>
-    <t>80.0</t>
-  </si>
-  <si>
-    <t>-4.934682680261566</t>
-  </si>
-  <si>
-    <t>CC1=CC=C(C2=NC(CN3C=NC4=C(N)N=C(N)N=C43)=CS2)O1</t>
-  </si>
-  <si>
-    <t>-11</t>
-  </si>
-  <si>
-    <t>s-34-13231222-1282712-</t>
-  </si>
-  <si>
-    <t>-0.4913561101771579</t>
-  </si>
-  <si>
-    <t>0.27957378274795375</t>
-  </si>
-  <si>
-    <t>86.66666666666667</t>
-  </si>
-  <si>
-    <t>mac-x0161</t>
-  </si>
-  <si>
-    <t>-11.301190534074632</t>
-  </si>
-  <si>
-    <t>O=C1CSC2=CC(C(=O)OC3C4=CC=CC=C4CC3F)=CC=C2N1</t>
-  </si>
-  <si>
-    <t>mac-x0381</t>
-  </si>
-  <si>
-    <t>-13</t>
-  </si>
-  <si>
-    <t>s-11-11560436-10336618</t>
-  </si>
-  <si>
-    <t>-0.1817918306185008</t>
-  </si>
-  <si>
-    <t>0.9356611298969302</t>
-  </si>
-  <si>
-    <t>93.33333333333333</t>
-  </si>
-  <si>
-    <t>mac-x0213</t>
-  </si>
-  <si>
-    <t>-4.72658759608102</t>
-  </si>
-  <si>
-    <t>O=C(NC1C2=CC=CC=C2CC1C(=O)O)C3=CC=CC=C3</t>
-  </si>
-  <si>
-    <t>m-272610-18205366-9959790</t>
-  </si>
-  <si>
-    <t>3.4592744025353803</t>
-  </si>
-  <si>
-    <t>0.959524274488839</t>
-  </si>
-  <si>
-    <t>100.0</t>
-  </si>
-  <si>
-    <t>mac-x0398</t>
-  </si>
-  <si>
-    <t>72.64476245324299</t>
   </si>
 </sst>
 </file>
@@ -1022,6 +1070,120 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="53530500"/>
+          <a:ext cx="2857500" cy="2857500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>2857500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="57340500"/>
+          <a:ext cx="2857500" cy="2857500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>2857500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="61150500"/>
+          <a:ext cx="2857500" cy="2857500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>2857500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="64960500"/>
           <a:ext cx="2857500" cy="2857500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1319,7 +1481,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:M16"/>
+  <dimension ref="B1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1377,107 +1539,107 @@
         <v>14</v>
       </c>
       <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>17</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>19</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>20</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>21</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>22</v>
-      </c>
-      <c r="M2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="2:13" ht="300" customHeight="1">
       <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
         <v>24</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>25</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>26</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>27</v>
       </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>28</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>29</v>
-      </c>
-      <c r="I3" t="s">
-        <v>19</v>
       </c>
       <c r="J3" t="s">
         <v>30</v>
       </c>
       <c r="K3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="L3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" t="s">
         <v>22</v>
-      </c>
-      <c r="M3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="4" spans="2:13" ht="300" customHeight="1">
       <c r="B4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
       </c>
       <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" t="s">
         <v>34</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>35</v>
       </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>36</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>37</v>
       </c>
-      <c r="I4" t="s">
-        <v>19</v>
-      </c>
       <c r="J4" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="K4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="L4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" t="s">
         <v>22</v>
-      </c>
-      <c r="M4" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="300" customHeight="1">
@@ -1494,36 +1656,36 @@
         <v>42</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="G5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I5" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="J5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K5" t="s">
         <v>20</v>
       </c>
-      <c r="K5" t="s">
-        <v>45</v>
-      </c>
       <c r="L5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" t="s">
         <v>22</v>
-      </c>
-      <c r="M5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="6" spans="2:13" ht="300" customHeight="1">
       <c r="B6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
         <v>49</v>
@@ -1532,408 +1694,522 @@
         <v>50</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="G6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I6" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="J6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="K6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="L6" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" t="s">
         <v>22</v>
-      </c>
-      <c r="M6" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="7" spans="2:13" ht="300" customHeight="1">
       <c r="B7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="G7" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="H7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I7" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="J7" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="K7" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="L7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M7" t="s">
         <v>22</v>
-      </c>
-      <c r="M7" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="8" spans="2:13" ht="300" customHeight="1">
       <c r="B8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F8" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="G8" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="H8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I8" t="s">
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="J8" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="K8" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="L8" t="s">
+        <v>21</v>
+      </c>
+      <c r="M8" t="s">
         <v>22</v>
-      </c>
-      <c r="M8" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="9" spans="2:13" ht="300" customHeight="1">
       <c r="B9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="E9" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F9" t="s">
-        <v>16</v>
+        <v>74</v>
       </c>
       <c r="G9" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="H9" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I9" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
       <c r="J9" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="K9" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="L9" t="s">
+        <v>21</v>
+      </c>
+      <c r="M9" t="s">
         <v>22</v>
-      </c>
-      <c r="M9" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="10" spans="2:13" ht="300" customHeight="1">
       <c r="B10" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E10" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="F10" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="G10" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="H10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I10" t="s">
-        <v>19</v>
+        <v>82</v>
       </c>
       <c r="J10" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="K10" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="L10" t="s">
+        <v>21</v>
+      </c>
+      <c r="M10" t="s">
         <v>22</v>
-      </c>
-      <c r="M10" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="11" spans="2:13" ht="300" customHeight="1">
       <c r="B11" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C11" t="s">
-        <v>84</v>
+        <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="E11" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F11" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G11" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
       <c r="H11" t="s">
         <v>88</v>
       </c>
       <c r="I11" t="s">
-        <v>19</v>
+        <v>89</v>
       </c>
       <c r="J11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="K11" t="s">
-        <v>90</v>
+        <v>56</v>
       </c>
       <c r="L11" t="s">
-        <v>91</v>
+        <v>21</v>
       </c>
       <c r="M11" t="s">
-        <v>92</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="2:13" ht="300" customHeight="1">
       <c r="B12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>92</v>
+      </c>
+      <c r="E12" t="s">
         <v>93</v>
       </c>
-      <c r="C12" t="s">
+      <c r="F12" t="s">
         <v>94</v>
       </c>
-      <c r="D12" t="s">
-        <v>64</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="G12" t="s">
+        <v>52</v>
+      </c>
+      <c r="H12" t="s">
         <v>95</v>
       </c>
-      <c r="F12" t="s">
-        <v>86</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="I12" t="s">
         <v>96</v>
       </c>
-      <c r="H12" t="s">
+      <c r="J12" t="s">
         <v>97</v>
       </c>
-      <c r="I12" t="s">
-        <v>19</v>
-      </c>
-      <c r="J12" t="s">
-        <v>98</v>
-      </c>
       <c r="K12" t="s">
-        <v>99</v>
+        <v>56</v>
       </c>
       <c r="L12" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="M12" t="s">
-        <v>101</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="2:13" ht="300" customHeight="1">
       <c r="B13" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>99</v>
+      </c>
+      <c r="E13" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" t="s">
+        <v>100</v>
+      </c>
+      <c r="G13" t="s">
+        <v>101</v>
+      </c>
+      <c r="H13" t="s">
         <v>102</v>
       </c>
-      <c r="C13" t="s">
-        <v>100</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="I13" t="s">
         <v>103</v>
       </c>
-      <c r="E13" t="s">
+      <c r="J13" t="s">
         <v>104</v>
       </c>
-      <c r="F13" t="s">
-        <v>86</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="K13" t="s">
         <v>105</v>
       </c>
-      <c r="H13" t="s">
-        <v>106</v>
-      </c>
-      <c r="I13" t="s">
-        <v>19</v>
-      </c>
-      <c r="J13" t="s">
-        <v>89</v>
-      </c>
-      <c r="K13" t="s">
-        <v>107</v>
-      </c>
       <c r="L13" t="s">
-        <v>94</v>
+        <v>21</v>
       </c>
       <c r="M13" t="s">
-        <v>108</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="2:13" ht="300" customHeight="1">
       <c r="B14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>107</v>
+      </c>
+      <c r="E14" t="s">
+        <v>108</v>
+      </c>
+      <c r="F14" t="s">
         <v>109</v>
       </c>
-      <c r="C14" t="s">
-        <v>84</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="G14" t="s">
+        <v>101</v>
+      </c>
+      <c r="H14" t="s">
         <v>110</v>
       </c>
-      <c r="E14" t="s">
+      <c r="I14" t="s">
         <v>111</v>
       </c>
-      <c r="F14" t="s">
-        <v>86</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="J14" t="s">
         <v>112</v>
       </c>
-      <c r="H14" t="s">
+      <c r="K14" t="s">
         <v>113</v>
       </c>
-      <c r="I14" t="s">
-        <v>19</v>
-      </c>
-      <c r="J14" t="s">
-        <v>89</v>
-      </c>
-      <c r="K14" t="s">
-        <v>114</v>
-      </c>
       <c r="L14" t="s">
-        <v>115</v>
+        <v>21</v>
       </c>
       <c r="M14" t="s">
-        <v>116</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="2:13" ht="300" customHeight="1">
       <c r="B15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>115</v>
+      </c>
+      <c r="E15" t="s">
+        <v>108</v>
+      </c>
+      <c r="F15" t="s">
+        <v>116</v>
+      </c>
+      <c r="G15" t="s">
         <v>117</v>
       </c>
-      <c r="C15" t="s">
+      <c r="H15" t="s">
         <v>118</v>
       </c>
-      <c r="D15" t="s">
+      <c r="I15" t="s">
         <v>119</v>
       </c>
-      <c r="E15" t="s">
+      <c r="J15" t="s">
         <v>120</v>
       </c>
-      <c r="F15" t="s">
-        <v>86</v>
-      </c>
-      <c r="G15" t="s">
-        <v>121</v>
-      </c>
-      <c r="H15" t="s">
-        <v>122</v>
-      </c>
-      <c r="I15" t="s">
-        <v>19</v>
-      </c>
-      <c r="J15" t="s">
-        <v>89</v>
-      </c>
       <c r="K15" t="s">
-        <v>123</v>
+        <v>20</v>
       </c>
       <c r="L15" t="s">
-        <v>124</v>
+        <v>21</v>
       </c>
       <c r="M15" t="s">
-        <v>125</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="2:13" ht="300" customHeight="1">
       <c r="B16" t="s">
+        <v>121</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
+        <v>122</v>
+      </c>
+      <c r="E16" t="s">
+        <v>108</v>
+      </c>
+      <c r="F16" t="s">
+        <v>123</v>
+      </c>
+      <c r="G16" t="s">
+        <v>124</v>
+      </c>
+      <c r="H16" t="s">
+        <v>125</v>
+      </c>
+      <c r="I16" t="s">
         <v>126</v>
       </c>
-      <c r="C16" t="s">
-        <v>124</v>
-      </c>
-      <c r="D16" t="s">
-        <v>103</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="J16" t="s">
         <v>127</v>
       </c>
-      <c r="F16" t="s">
-        <v>86</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="K16" t="s">
+        <v>20</v>
+      </c>
+      <c r="L16" t="s">
+        <v>21</v>
+      </c>
+      <c r="M16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" ht="300" customHeight="1">
+      <c r="B17" t="s">
         <v>128</v>
       </c>
-      <c r="H16" t="s">
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" t="s">
         <v>129</v>
       </c>
-      <c r="I16" t="s">
-        <v>19</v>
-      </c>
-      <c r="J16" t="s">
-        <v>89</v>
-      </c>
-      <c r="K16" t="s">
+      <c r="E17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" t="s">
         <v>130</v>
       </c>
-      <c r="L16" t="s">
+      <c r="G17" t="s">
+        <v>117</v>
+      </c>
+      <c r="H17" t="s">
         <v>131</v>
       </c>
-      <c r="M16" t="s">
+      <c r="I17" t="s">
         <v>132</v>
+      </c>
+      <c r="J17" t="s">
+        <v>133</v>
+      </c>
+      <c r="K17" t="s">
+        <v>20</v>
+      </c>
+      <c r="L17" t="s">
+        <v>21</v>
+      </c>
+      <c r="M17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" ht="300" customHeight="1">
+      <c r="B18" t="s">
+        <v>134</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
+        <v>135</v>
+      </c>
+      <c r="E18" t="s">
+        <v>136</v>
+      </c>
+      <c r="F18" t="s">
+        <v>137</v>
+      </c>
+      <c r="G18" t="s">
+        <v>138</v>
+      </c>
+      <c r="H18" t="s">
+        <v>139</v>
+      </c>
+      <c r="I18" t="s">
+        <v>140</v>
+      </c>
+      <c r="J18" t="s">
+        <v>141</v>
+      </c>
+      <c r="K18" t="s">
+        <v>56</v>
+      </c>
+      <c r="L18" t="s">
+        <v>21</v>
+      </c>
+      <c r="M18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" ht="300" customHeight="1">
+      <c r="B19" t="s">
+        <v>142</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" t="s">
+        <v>143</v>
+      </c>
+      <c r="E19" t="s">
+        <v>108</v>
+      </c>
+      <c r="F19" t="s">
+        <v>144</v>
+      </c>
+      <c r="G19" t="s">
+        <v>145</v>
+      </c>
+      <c r="H19" t="s">
+        <v>146</v>
+      </c>
+      <c r="I19" t="s">
+        <v>147</v>
+      </c>
+      <c r="J19" t="s">
+        <v>148</v>
+      </c>
+      <c r="K19" t="s">
+        <v>39</v>
+      </c>
+      <c r="L19" t="s">
+        <v>21</v>
+      </c>
+      <c r="M19" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>